<commit_message>
last known working frequency measure
</commit_message>
<xml_diff>
--- a/algorithm proto/results.xlsx
+++ b/algorithm proto/results.xlsx
@@ -8,21 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Desktop\school\capstone\capstone code\algorithm proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BD360D-7BF0-403A-A48C-D667AAB53F5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABEC565-A827-45CB-8578-BF55FCB52844}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0FE87E-33D9-4A6C-ACD6-13EF39E57134}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="frequency" sheetId="1" r:id="rId1"/>
+    <sheet name="area" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$2:$J$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$3:$J$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$4:$J$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$5:$J$5</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$6:$J$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$7:$J$7</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>size</t>
   </si>
@@ -54,6 +47,54 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>eccentricity</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>measured area</t>
+  </si>
+  <si>
+    <t>trial</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m3</t>
   </si>
 </sst>
 </file>
@@ -89,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,7 +227,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$J$2</c:f>
+              <c:f>frequency!$C$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -218,7 +260,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$J$3</c:f>
+              <c:f>frequency!$C$3:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -259,7 +301,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$J$2</c:f>
+              <c:f>frequency!$C$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -292,7 +334,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$J$4</c:f>
+              <c:f>frequency!$C$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -357,7 +399,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$J$2</c:f>
+              <c:f>frequency!$C$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -390,7 +432,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$J$5</c:f>
+              <c:f>frequency!$C$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -615,7 +657,1345 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>m1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38354903364352183"/>
+                  <c:y val="-0.14460270857037202"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>area!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.10367255756846318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17310175521279758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2938046054770537E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11875220230569418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23876104167282428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>area!$M$3:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.0698972735128291E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7805766520230006E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7780350763794133E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1282480470246838E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D24A-45BF-AE9F-AE3A4644C468}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="429769264"/>
+        <c:axId val="440901752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="429769264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440901752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="440901752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429769264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>m2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38354903364352183"/>
+                  <c:y val="-0.14460270857037202"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>area!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.10367255756846318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17310175521279758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2938046054770537E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11875220230569418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23876104167282428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>area!$M$8:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.0702420045509967E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8645797469753964E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1600796477581163E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8694431737785601E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2548770994245789E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8F82-4ECA-BD08-6DAEE9985089}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="429769264"/>
+        <c:axId val="440901752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="429769264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440901752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="440901752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429769264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>m3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38354903364352183"/>
+                  <c:y val="-0.14460270857037202"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>area!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.10367255756846318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17310175521279758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2938046054770537E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11875220230569418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23876104167282428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>area!$M$13:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.302477441456318E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5566655190321277E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0112254872825993E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9822181560913866E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2156067181586597E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8675-4EC0-917F-658167EC80E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="429769264"/>
+        <c:axId val="440901752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="429769264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440901752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="440901752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429769264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1171,6 +2551,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1204,6 +4132,123 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F5E4BB3-9FC0-4512-8867-77B250CDFEF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178FD523-1371-472E-874C-7E23EB8D8DE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>128588</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16CE12F9-375B-4909-9413-29106CA92C2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1512,7 +4557,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,4 +4771,439 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CADB7BF-E40A-4E7D-9885-3466BD86851C}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0.33</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <f>PI()*C3*B3</f>
+        <v>0.10367255756846318</v>
+      </c>
+      <c r="E3">
+        <f>SQRT(1-C3^2/B3^2)</f>
+        <v>0.95298092081917507</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1">
+        <v>9.1691110647597896E-5</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1.8040580755778699E-4</v>
+      </c>
+      <c r="M3">
+        <f>AVERAGE(I3:K3)</f>
+        <v>9.0698972735128291E-5</v>
+      </c>
+      <c r="N3">
+        <f>_xlfn.STDEV.S(I3:K3)</f>
+        <v>9.0206995867129602E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.19</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="0">PI()*C4*B4</f>
+        <v>0.17310175521279758</v>
+      </c>
+      <c r="E4">
+        <f>SQRT(1-C4^2/B4^2)</f>
+        <v>0.75547938966229811</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M7" si="1">AVERAGE(I4:K4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N7" si="2">_xlfn.STDEV.S(I4:K4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.24</v>
+      </c>
+      <c r="C5">
+        <v>0.11</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.2938046054770537E-2</v>
+      </c>
+      <c r="E5">
+        <f>SQRT(1-C5^2/B5^2)</f>
+        <v>0.8887803753208976</v>
+      </c>
+      <c r="I5">
+        <v>1.7341729956069001E-4</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>5.7805766520230006E-5</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>1.0012252458350234E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0.21</v>
+      </c>
+      <c r="C6">
+        <v>0.18</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.11875220230569418</v>
+      </c>
+      <c r="E6">
+        <f>SQRT(1-C6^2/B6^2)</f>
+        <v>0.51507875363771272</v>
+      </c>
+      <c r="I6">
+        <v>5.3341052291382401E-3</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>1.7780350763794133E-3</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>3.0796470899287533E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0.38</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.23876104167282428</v>
+      </c>
+      <c r="E7">
+        <f>SQRT(1-C7^2/B7^2)</f>
+        <v>0.850289180073869</v>
+      </c>
+      <c r="I7" s="1">
+        <v>9.70938001811509E-5</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1.22876503408929E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>4.1282480470246838E-3</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>7.0664164288835136E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8">
+        <v>1.9770597947514801E-3</v>
+      </c>
+      <c r="J8">
+        <v>3.8460173034688501E-3</v>
+      </c>
+      <c r="K8">
+        <v>6.3876489154326603E-3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:M17" si="3">AVERAGE(I8:K8)</f>
+        <v>4.0702420045509967E-3</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:N17" si="4">_xlfn.STDEV.S(I8:K8)</f>
+        <v>2.2138273725156024E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>8.0834275471054003E-4</v>
+      </c>
+      <c r="J9">
+        <v>5.1816823329628101E-3</v>
+      </c>
+      <c r="K9">
+        <v>8.6037141532528394E-3</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>4.8645797469753964E-3</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>3.907348122170938E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>2.59598650118534E-3</v>
+      </c>
+      <c r="J10">
+        <v>3.5497504386596801E-3</v>
+      </c>
+      <c r="K10">
+        <v>3.3345020034293302E-3</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>3.1600796477581163E-3</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>5.0023372609717218E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1.39808418845707E-2</v>
+      </c>
+      <c r="J11">
+        <v>2.1008759089641199E-2</v>
+      </c>
+      <c r="K11">
+        <v>2.1093694239144901E-2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>1.8694431737785601E-2</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>4.0823094533796863E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>6.66515698102746E-3</v>
+      </c>
+      <c r="J12">
+        <v>1.9581644393162098E-3</v>
+      </c>
+      <c r="K12">
+        <v>5.9022991562393698E-2</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>2.2548770994245789E-2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>3.167515618331438E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>6.3265913432047401E-3</v>
+      </c>
+      <c r="J13">
+        <v>1.2307255371100299E-2</v>
+      </c>
+      <c r="K13">
+        <v>2.0440476529384501E-2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>1.302477441456318E-2</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>7.0842475920499135E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>2.5866968150737302E-3</v>
+      </c>
+      <c r="J14">
+        <v>1.6581383465480999E-2</v>
+      </c>
+      <c r="K14">
+        <v>2.7531885290409099E-2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>1.5566655190321277E-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>1.2503513990947008E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>8.3071568037930803E-3</v>
+      </c>
+      <c r="J15">
+        <v>1.1359201403711E-2</v>
+      </c>
+      <c r="K15">
+        <v>1.0670406410973899E-2</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>1.0112254872825993E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>1.6007479235109719E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>4.4738694030626198E-2</v>
+      </c>
+      <c r="J16">
+        <v>6.7228029086851701E-2</v>
+      </c>
+      <c r="K16">
+        <v>6.7499821565263698E-2</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>5.9822181560913866E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>1.3063390250815E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>2.1328502339287899E-2</v>
+      </c>
+      <c r="J17">
+        <v>6.26612620581188E-3</v>
+      </c>
+      <c r="K17">
+        <v>0.18887357299966001</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>7.2156067181586597E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>0.10136049978660611</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
activity classifier proto completed
</commit_message>
<xml_diff>
--- a/algorithm proto/results.xlsx
+++ b/algorithm proto/results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Desktop\school\capstone\capstone code\algorithm proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABEC565-A827-45CB-8578-BF55FCB52844}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F5CE16-C40B-4ABF-8009-CBADA81F5CF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0FE87E-33D9-4A6C-ACD6-13EF39E57134}"/>
+    <workbookView xWindow="28680" yWindow="1560" windowWidth="20730" windowHeight="11160" xr2:uid="{5F0FE87E-33D9-4A6C-ACD6-13EF39E57134}"/>
   </bookViews>
   <sheets>
     <sheet name="frequency" sheetId="1" r:id="rId1"/>
     <sheet name="area" sheetId="2" r:id="rId2"/>
+    <sheet name="activity times" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>size</t>
   </si>
@@ -96,6 +97,42 @@
   <si>
     <t>m3</t>
   </si>
+  <si>
+    <t>m4</t>
+  </si>
+  <si>
+    <t>3 roommates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">window (seconds) </t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>active t (min)</t>
+  </si>
+  <si>
+    <t>inactive t (min)</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>working at desk</t>
+  </si>
+  <si>
+    <t>cooking</t>
+  </si>
+  <si>
+    <t>moving around room to get things</t>
+  </si>
+  <si>
+    <t>titles</t>
+  </si>
+  <si>
+    <t>stdev</t>
+  </si>
 </sst>
 </file>
 
@@ -118,9 +155,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -130,9 +176,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,28 +386,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.9851180881350801</c:v>
+                  <c:v>1.99729852735407</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9789035803178201</c:v>
+                  <c:v>1.99752457209156</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.54979062551807</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.478073722682</c:v>
+                  <c:v>1.4979878896043699</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0041127468914399</c:v>
+                  <c:v>0.99857167619708098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.96838985694941304</c:v>
+                  <c:v>0.99897184186413401</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.22800187233935201</c:v>
+                  <c:v>0.49923763264724302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68272611380339998</c:v>
+                  <c:v>0.499452918716908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,28 +484,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.0269129436259301</c:v>
+                  <c:v>1.9972442245575599</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.00587260674684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5262150524318701</c:v>
+                  <c:v>1.4975517866132</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5054790951119701</c:v>
+                  <c:v>1.4978511494435001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.00535569580512</c:v>
+                  <c:v>0.99893169774885604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97550431478145905</c:v>
+                  <c:v>0.99839969445937804</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.52035563329768197</c:v>
+                  <c:v>0.59903215869149296</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.50540244401992596</c:v>
+                  <c:v>0.49919209712172702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -672,6 +719,378 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(frequency!$D$8,frequency!$F$8,frequency!$H$8,frequency!$J$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.2601461144781607E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.5997479709529869E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.7858533996331399E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.9869100992872242E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(frequency!$D$8,frequency!$F$8,frequency!$H$8,frequency!$J$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.2601461144781607E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.5997479709529869E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.7858533996331399E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.9869100992872242E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(frequency!$D$2,frequency!$F$2,frequency!$H$2,frequency!$J$2)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(frequency!$C$8,frequency!$E$8,frequency!$G$8,frequency!$I$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.9994849826875072</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.510795362794785</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99871872756736235</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52422870179434278</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A650-40AB-A3A0-66FCAA4BD367}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="311094200"/>
+        <c:axId val="304075248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="311094200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="304075248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="304075248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="311094200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -821,6 +1240,73 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>area!$N$3:$N$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>2.9852861559904471E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.242542799922063E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.15991590650146029</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.6171764596590086E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.5717040250111662E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>area!$N$3:$N$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>2.9852861559904471E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.242542799922063E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.15991590650146029</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.6171764596590086E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.5717040250111662E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>area!$D$3:$D$7</c:f>
@@ -852,19 +1338,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.0698972735128291E-5</c:v>
+                  <c:v>2.64159045783104E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.5166828370332534E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7805766520230006E-5</c:v>
+                  <c:v>0.1198935178889986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7780350763794133E-3</c:v>
+                  <c:v>6.8182330964144097E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1282480470246838E-3</c:v>
+                  <c:v>7.9485321298270462E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,412 +1359,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D24A-45BF-AE9F-AE3A4644C468}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="429769264"/>
-        <c:axId val="440901752"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="429769264"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="440901752"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="440901752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="429769264"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>m2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.38354903364352183"/>
-                  <c:y val="-0.14460270857037202"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>area!$D$3:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.10367255756846318</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.17310175521279758</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.2938046054770537E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11875220230569418</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.23876104167282428</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>area!$M$8:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.0702420045509967E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.8645797469753964E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.1600796477581163E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8694431737785601E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.2548770994245789E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8F82-4ECA-BD08-6DAEE9985089}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1504,6 +1584,412 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>m2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38354903364352183"/>
+                  <c:y val="-0.14460270857037202"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>area!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.10367255756846318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17310175521279758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2938046054770537E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11875220230569418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23876104167282428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>area!$M$8:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.12182626327719263</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22459059185321084</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9096298315322226E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13400519800777091</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16795501085960898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8F82-4ECA-BD08-6DAEE9985089}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="429769264"/>
+        <c:axId val="440901752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="429769264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440901752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="440901752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429769264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>m3</a:t>
             </a:r>
           </a:p>
@@ -1664,19 +2150,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.302477441456318E-2</c:v>
+                  <c:v>0.38984404248701598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5566655190321277E-2</c:v>
+                  <c:v>0.71868989393027372</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0112254872825993E-2</c:v>
+                  <c:v>0.3171081546090313</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9822181560913866E-2</c:v>
+                  <c:v>0.42881663362486733</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2156067181586597E-2</c:v>
+                  <c:v>0.53745603475074799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1685,6 +2171,420 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8675-4EC0-917F-658167EC80E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="429769264"/>
+        <c:axId val="440901752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="429769264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440901752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="440901752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429769264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>m4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46293450151612298"/>
+          <c:y val="3.8369298760278892E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38354903364352183"/>
+                  <c:y val="-0.14460270857037202"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>area!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.10367255756846318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17310175521279758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2938046054770537E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11875220230569418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23876104167282428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>area!$M$18:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.46175821769629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87907257425779306</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35724847276072597</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9467504972980666E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.278209014309591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-48AC-4C05-AC6D-48073817F42D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2035,6 +2935,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3584,6 +4564,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4104,15 +6116,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4137,6 +6149,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBDC80A6-034D-4B12-9539-127FAD6DBACE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4144,15 +6192,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>17368</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>550768</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4180,16 +6228,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>372034</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>135312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4218,16 +6266,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>146797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>528917</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>27735</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4249,6 +6297,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>246528</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>170328</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>105056</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC5B3A5-B0FB-4CAC-9B88-C03D8224F299}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4554,20 +6640,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BEB1C7-23DE-4E3D-B78C-B06148BA2880}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -4596,75 +6682,135 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>1.9851180881350801</v>
+        <v>1.99729852735407</v>
       </c>
       <c r="D4">
-        <v>1.9789035803178201</v>
+        <v>1.99752457209156</v>
       </c>
       <c r="E4">
         <v>1.54979062551807</v>
       </c>
       <c r="F4">
-        <v>1.478073722682</v>
+        <v>1.4979878896043699</v>
       </c>
       <c r="G4">
-        <v>1.0041127468914399</v>
+        <v>0.99857167619708098</v>
       </c>
       <c r="H4">
-        <v>0.96838985694941304</v>
+        <v>0.99897184186413401</v>
       </c>
       <c r="I4">
-        <v>0.22800187233935201</v>
+        <v>0.49923763264724302</v>
       </c>
       <c r="J4">
-        <v>0.68272611380339998</v>
+        <v>0.499452918716908</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.2</v>
       </c>
       <c r="C5">
-        <v>2.0269129436259301</v>
+        <v>1.9972442245575599</v>
       </c>
       <c r="D5">
         <v>2.00587260674684</v>
       </c>
       <c r="E5">
-        <v>1.5262150524318701</v>
+        <v>1.4975517866132</v>
       </c>
       <c r="F5">
-        <v>1.5054790951119701</v>
+        <v>1.4978511494435001</v>
       </c>
       <c r="G5">
-        <v>1.00535569580512</v>
+        <v>0.99893169774885604</v>
       </c>
       <c r="H5">
-        <v>0.97550431478145905</v>
+        <v>0.99839969445937804</v>
       </c>
       <c r="I5">
-        <v>0.52035563329768197</v>
+        <v>0.59903215869149296</v>
       </c>
       <c r="J5">
-        <v>0.50540244401992596</v>
+        <v>0.49919209712172702</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f>AVERAGE(C4:D5)</f>
+        <v>1.9994849826875072</v>
+      </c>
+      <c r="D8">
+        <f>_xlfn.STDEV.S(C4:D5)</f>
+        <v>4.2601461144781607E-3</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(E4:F5)</f>
+        <v>1.510795362794785</v>
+      </c>
+      <c r="F8">
+        <f>_xlfn.STDEV.S(E4:F5)</f>
+        <v>2.5997479709529869E-2</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(G4:H5)</f>
+        <v>0.99871872756736235</v>
+      </c>
+      <c r="H8">
+        <f>_xlfn.STDEV.S(G4:H5)</f>
+        <v>2.7858533996331399E-4</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(I4:J5)</f>
+        <v>0.52422870179434278</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.STDEV.S(I4:J5)</f>
+        <v>4.9869100992872242E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -4695,76 +6841,87 @@
       <c r="L13" t="s">
         <v>4</v>
       </c>
+      <c r="M13" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.15</v>
       </c>
       <c r="C15">
-        <v>0.32078309584144299</v>
+        <v>0.11185308140507499</v>
       </c>
       <c r="D15">
-        <v>0.336428796044629</v>
+        <v>0.148582332392486</v>
       </c>
       <c r="E15">
-        <v>0.40588688978553</v>
+        <v>0.11762309528182301</v>
       </c>
       <c r="F15">
-        <v>0.41482621115102097</v>
+        <v>0.104000651957134</v>
       </c>
       <c r="G15">
-        <v>0.30496615144898498</v>
+        <v>7.7418419997048196E-2</v>
       </c>
       <c r="H15">
-        <v>0.13973116347546299</v>
+        <v>8.6519639501003498E-2</v>
       </c>
       <c r="I15">
-        <v>0.18804015971167701</v>
+        <v>7.3209066529601394E-2</v>
       </c>
       <c r="J15">
-        <v>6.5851216144680605E-2</v>
+        <v>7.9405002277462694E-2</v>
       </c>
       <c r="L15">
         <f>AVERAGE(C15:J15)</f>
-        <v>0.27206421045042861</v>
+        <v>9.9826411167704215E-2</v>
+      </c>
+      <c r="M15">
+        <f>_xlfn.STDEV.S(C15:J15)</f>
+        <v>2.5803189504514903E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.2</v>
       </c>
       <c r="C16">
-        <v>0.39999250335073799</v>
+        <v>0.20324739328816499</v>
       </c>
       <c r="D16">
-        <v>0.43373750654495202</v>
+        <v>0.147951794025831</v>
       </c>
       <c r="E16">
-        <v>0.49355363004489899</v>
+        <v>0.137534467511638</v>
       </c>
       <c r="F16">
-        <v>0.52672397344598598</v>
+        <v>0.12911967027597901</v>
       </c>
       <c r="G16">
-        <v>0.211631162777594</v>
+        <v>0.13894935880112</v>
       </c>
       <c r="H16">
-        <v>0.35014628847981599</v>
+        <v>0.11788376523397499</v>
       </c>
       <c r="I16">
-        <v>0.201324613020715</v>
+        <v>0.219155547315281</v>
       </c>
       <c r="J16">
-        <v>6.5917499423499198E-2</v>
+        <v>0.1217439510153</v>
       </c>
       <c r="L16">
         <f>AVERAGE(C16:J16)</f>
-        <v>0.33537839713602496</v>
+        <v>0.15194824343341115</v>
+      </c>
+      <c r="M16">
+        <f>_xlfn.STDEV.S(C16:J16)</f>
+        <v>3.8050634919890143E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4775,10 +6932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CADB7BF-E40A-4E7D-9885-3466BD86851C}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,21 +7002,21 @@
         <v>18</v>
       </c>
       <c r="I3" s="1">
-        <v>9.1691110647597896E-5</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>5.8803099091730399E-2</v>
       </c>
       <c r="K3">
-        <v>1.8040580755778699E-4</v>
+        <v>2.0444614643200801E-2</v>
       </c>
       <c r="M3">
         <f>AVERAGE(I3:K3)</f>
-        <v>9.0698972735128291E-5</v>
+        <v>2.64159045783104E-2</v>
       </c>
       <c r="N3">
         <f>_xlfn.STDEV.S(I3:K3)</f>
-        <v>9.0206995867129602E-5</v>
+        <v>2.9852861559904471E-2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4880,22 +7037,22 @@
         <f>SQRT(1-C4^2/B4^2)</f>
         <v>0.75547938966229811</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1.37422971359859E-2</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>6.1758187975011702E-2</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M7" si="1">AVERAGE(I4:K4)</f>
-        <v>0</v>
+        <v>2.5166828370332534E-2</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N7" si="2">_xlfn.STDEV.S(I4:K4)</f>
-        <v>0</v>
+        <v>3.242542799922063E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4916,22 +7073,22 @@
         <f>SQRT(1-C5^2/B5^2)</f>
         <v>0.8887803753208976</v>
       </c>
-      <c r="I5">
-        <v>1.7341729956069001E-4</v>
+      <c r="I5" s="1">
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.30146369328088302</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>5.8216860386112797E-2</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>5.7805766520230006E-5</v>
+        <v>0.1198935178889986</v>
       </c>
       <c r="N5">
         <f t="shared" si="2"/>
-        <v>1.0012252458350234E-4</v>
+        <v>0.15991590650146029</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4953,21 +7110,21 @@
         <v>0.51507875363771272</v>
       </c>
       <c r="I6">
-        <v>5.3341052291382401E-3</v>
+        <v>4.7966025082413398E-2</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>5.8837026770825002E-2</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>9.7743941039193899E-2</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>1.7780350763794133E-3</v>
+        <v>6.8182330964144097E-2</v>
       </c>
       <c r="N6">
         <f t="shared" si="2"/>
-        <v>3.0796470899287533E-3</v>
+        <v>2.6171764596590086E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4989,21 +7146,21 @@
         <v>0.850289180073869</v>
       </c>
       <c r="I7" s="1">
-        <v>9.70938001811509E-5</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>6.8149867624123395E-2</v>
       </c>
       <c r="K7">
-        <v>1.22876503408929E-2</v>
+        <v>0.17030609627068799</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>4.1282480470246838E-3</v>
+        <v>7.9485321298270462E-2</v>
       </c>
       <c r="N7">
         <f t="shared" si="2"/>
-        <v>7.0664164288835136E-3</v>
+        <v>8.5717040250111662E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5011,97 +7168,97 @@
         <v>19</v>
       </c>
       <c r="I8">
-        <v>1.9770597947514801E-3</v>
+        <v>0.152156069189506</v>
       </c>
       <c r="J8">
-        <v>3.8460173034688501E-3</v>
+        <v>0.16230101907674099</v>
       </c>
       <c r="K8">
-        <v>6.3876489154326603E-3</v>
+        <v>5.1021701565330903E-2</v>
       </c>
       <c r="M8">
         <f t="shared" ref="M8:M17" si="3">AVERAGE(I8:K8)</f>
-        <v>4.0702420045509967E-3</v>
+        <v>0.12182626327719263</v>
       </c>
       <c r="N8">
         <f t="shared" ref="N8:N17" si="4">_xlfn.STDEV.S(I8:K8)</f>
-        <v>2.2138273725156024E-3</v>
+        <v>6.1527997460182754E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I9">
-        <v>8.0834275471054003E-4</v>
+        <v>0.540446765234601</v>
       </c>
       <c r="J9">
-        <v>5.1816823329628101E-3</v>
+        <v>5.9092315117220802E-2</v>
       </c>
       <c r="K9">
-        <v>8.6037141532528394E-3</v>
+        <v>7.4232695207810701E-2</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>4.8645797469753964E-3</v>
+        <v>0.22459059185321084</v>
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
-        <v>3.907348122170938E-3</v>
+        <v>0.27364420234069087</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I10">
-        <v>2.59598650118534E-3</v>
+        <v>5.2736832879831698E-2</v>
       </c>
       <c r="J10">
-        <v>3.5497504386596801E-3</v>
+        <v>0.114068290971389</v>
       </c>
       <c r="K10">
-        <v>3.3345020034293302E-3</v>
+        <v>0.13048377109474599</v>
       </c>
       <c r="M10">
         <f t="shared" si="3"/>
-        <v>3.1600796477581163E-3</v>
+        <v>9.9096298315322226E-2</v>
       </c>
       <c r="N10">
         <f t="shared" si="4"/>
-        <v>5.0023372609717218E-4</v>
+        <v>4.0978860690829538E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I11">
-        <v>1.39808418845707E-2</v>
+        <v>0.124733202579952</v>
       </c>
       <c r="J11">
-        <v>2.1008759089641199E-2</v>
+        <v>8.4399691218667694E-2</v>
       </c>
       <c r="K11">
-        <v>2.1093694239144901E-2</v>
+        <v>0.192882700224693</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>1.8694431737785601E-2</v>
+        <v>0.13400519800777091</v>
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>4.0823094533796863E-3</v>
+        <v>5.4832638411446699E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I12">
-        <v>6.66515698102746E-3</v>
+        <v>0.14161660111966401</v>
       </c>
       <c r="J12">
-        <v>1.9581644393162098E-3</v>
+        <v>0.14642712952341899</v>
       </c>
       <c r="K12">
-        <v>5.9022991562393698E-2</v>
+        <v>0.215821301935744</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
-        <v>2.2548770994245789E-2</v>
+        <v>0.16795501085960898</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>3.167515618331438E-2</v>
+        <v>4.1523146098529196E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -5109,101 +7266,287 @@
         <v>20</v>
       </c>
       <c r="I13">
-        <v>6.3265913432047401E-3</v>
+        <v>0.48689942140641901</v>
       </c>
       <c r="J13">
-        <v>1.2307255371100299E-2</v>
+        <v>0.51936326104556996</v>
       </c>
       <c r="K13">
-        <v>2.0440476529384501E-2</v>
+        <v>0.16326944500905899</v>
       </c>
       <c r="M13">
         <f t="shared" si="3"/>
-        <v>1.302477441456318E-2</v>
+        <v>0.38984404248701598</v>
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>7.0842475920499135E-3</v>
+        <v>0.1968895918725842</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I14">
-        <v>2.5866968150737302E-3</v>
+        <v>1.7294296487507199</v>
       </c>
       <c r="J14">
-        <v>1.6581383465480999E-2</v>
+        <v>0.18909540837510699</v>
       </c>
       <c r="K14">
-        <v>2.7531885290409099E-2</v>
+        <v>0.23754462466499399</v>
       </c>
       <c r="M14">
         <f t="shared" si="3"/>
-        <v>1.5566655190321277E-2</v>
+        <v>0.71868989393027372</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>1.2503513990947008E-2</v>
+        <v>0.87566144749020891</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I15">
-        <v>8.3071568037930803E-3</v>
+        <v>0.16875786521546199</v>
       </c>
       <c r="J15">
-        <v>1.1359201403711E-2</v>
+        <v>0.36501853110844601</v>
       </c>
       <c r="K15">
-        <v>1.0670406410973899E-2</v>
+        <v>0.41754806750318602</v>
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
-        <v>1.0112254872825993E-2</v>
+        <v>0.3171081546090313</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>1.6007479235109719E-3</v>
+        <v>0.13113235421065403</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I16">
-        <v>4.4738694030626198E-2</v>
+        <v>0.39914624825584599</v>
       </c>
       <c r="J16">
-        <v>6.7228029086851701E-2</v>
+        <v>0.27007901189973699</v>
       </c>
       <c r="K16">
-        <v>6.7499821565263698E-2</v>
+        <v>0.61722464071901895</v>
       </c>
       <c r="M16">
         <f t="shared" si="3"/>
-        <v>5.9822181560913866E-2</v>
+        <v>0.42881663362486733</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>1.3063390250815E-2</v>
+        <v>0.1754644429166301</v>
       </c>
     </row>
-    <row r="17" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
       <c r="I17">
-        <v>2.1328502339287899E-2</v>
+        <v>0.453173123582924</v>
       </c>
       <c r="J17">
-        <v>6.26612620581188E-3</v>
+        <v>0.46856681447494097</v>
       </c>
       <c r="K17">
-        <v>0.18887357299966001</v>
+        <v>0.69062816619437895</v>
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
-        <v>7.2156067181586597E-2</v>
+        <v>0.53745603475074799</v>
       </c>
       <c r="N17">
         <f t="shared" si="4"/>
-        <v>0.10136049978660611</v>
+        <v>0.13287406751529232</v>
+      </c>
+    </row>
+    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18">
+        <v>0.680090408191806</v>
+      </c>
+      <c r="J18">
+        <v>0.64890329911718103</v>
+      </c>
+      <c r="K18">
+        <v>5.6280945779882997E-2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M22" si="5">AVERAGE(I18:K18)</f>
+        <v>0.46175821769629</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:N22" si="6">_xlfn.STDEV.S(I18:K18)</f>
+        <v>0.35149967634933477</v>
+      </c>
+    </row>
+    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>2.4164511830418798</v>
+      </c>
+      <c r="J19">
+        <v>0.17950904182923799</v>
+      </c>
+      <c r="K19">
+        <v>4.12574979022612E-2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="5"/>
+        <v>0.87907257425779306</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="6"/>
+        <v>1.3332022023720629</v>
+      </c>
+    </row>
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>0.110999907430572</v>
+      </c>
+      <c r="J20">
+        <v>0.84448158890081004</v>
+      </c>
+      <c r="K20">
+        <v>0.116263921950796</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="5"/>
+        <v>0.35724847276072597</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="6"/>
+        <v>0.42196446480704958</v>
+      </c>
+    </row>
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>4.4741729075789799E-2</v>
+      </c>
+      <c r="J21">
+        <v>7.2189470273408704E-2</v>
+      </c>
+      <c r="K21">
+        <v>6.1471315569743501E-2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="5"/>
+        <v>5.9467504972980666E-2</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="6"/>
+        <v>1.3833151011018457E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>0.41025680321013802</v>
+      </c>
+      <c r="J22">
+        <v>0.106137650482607</v>
+      </c>
+      <c r="K22">
+        <v>0.31823258923602799</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="5"/>
+        <v>0.278209014309591</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="6"/>
+        <v>0.15596002589236421</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79751478-6D87-483F-B9B5-B653690D23AE}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13" style="2" customWidth="1"/>
+    <col min="8" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="31" style="2" customWidth="1"/>
+    <col min="11" max="12" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <f>H2*60/E2</f>
+        <v>360</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <f>K2*60/E2</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added batch fft and classification to app
</commit_message>
<xml_diff>
--- a/algorithm proto/results.xlsx
+++ b/algorithm proto/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Desktop\school\capstone\capstone code\algorithm proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F5CE16-C40B-4ABF-8009-CBADA81F5CF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210FB5F8-C306-4CBC-A907-311887F7689A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1560" windowWidth="20730" windowHeight="11160" xr2:uid="{5F0FE87E-33D9-4A6C-ACD6-13EF39E57134}"/>
   </bookViews>
@@ -386,28 +386,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.99729852735407</c:v>
+                  <c:v>1.9851180881350801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.99752457209156</c:v>
+                  <c:v>1.9789035803178201</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.54979062551807</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4979878896043699</c:v>
+                  <c:v>1.478073722682</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99857167619708098</c:v>
+                  <c:v>1.0041127468914399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99897184186413401</c:v>
+                  <c:v>0.96838985694941304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49923763264724302</c:v>
+                  <c:v>0.41040337021083301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.499452918716908</c:v>
+                  <c:v>0.68272611380339998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,28 +484,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.9972442245575599</c:v>
+                  <c:v>2.0269129436259301</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.00587260674684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4975517866132</c:v>
+                  <c:v>1.5262150524318701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4978511494435001</c:v>
+                  <c:v>1.5054790951119701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99893169774885604</c:v>
+                  <c:v>1.00535569580512</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99839969445937804</c:v>
+                  <c:v>0.97550431478145905</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59903215869149296</c:v>
+                  <c:v>1.0081890395142601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.49919209712172702</c:v>
+                  <c:v>0.50540244401992596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,16 +791,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>4.2601461144781607E-3</c:v>
+                    <c:v>2.1777479237893492E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.5997479709529869E-2</c:v>
+                    <c:v>3.0497616737153389E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.7858533996331399E-4</c:v>
+                    <c:v>1.9157909326553625E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.9869100992872242E-2</c:v>
+                    <c:v>0.26310586709748757</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -812,16 +812,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>4.2601461144781607E-3</c:v>
+                    <c:v>2.1777479237893492E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.5997479709529869E-2</c:v>
+                    <c:v>3.0497616737153389E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.7858533996331399E-4</c:v>
+                    <c:v>1.9157909326553625E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.9869100992872242E-2</c:v>
+                    <c:v>0.26310586709748757</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -868,16 +868,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.9994849826875072</c:v>
+                  <c:v>1.9992018047064173</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.510795362794785</c:v>
+                  <c:v>1.5148896239359775</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99871872756736235</c:v>
+                  <c:v>0.98834065360685797</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52422870179434278</c:v>
+                  <c:v>0.65168024188710472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6643,7 +6643,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,28 +6692,28 @@
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>1.99729852735407</v>
+        <v>1.9851180881350801</v>
       </c>
       <c r="D4">
-        <v>1.99752457209156</v>
+        <v>1.9789035803178201</v>
       </c>
       <c r="E4">
         <v>1.54979062551807</v>
       </c>
       <c r="F4">
-        <v>1.4979878896043699</v>
+        <v>1.478073722682</v>
       </c>
       <c r="G4">
-        <v>0.99857167619708098</v>
+        <v>1.0041127468914399</v>
       </c>
       <c r="H4">
-        <v>0.99897184186413401</v>
+        <v>0.96838985694941304</v>
       </c>
       <c r="I4">
-        <v>0.49923763264724302</v>
+        <v>0.41040337021083301</v>
       </c>
       <c r="J4">
-        <v>0.499452918716908</v>
+        <v>0.68272611380339998</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6721,28 +6721,28 @@
         <v>0.2</v>
       </c>
       <c r="C5">
-        <v>1.9972442245575599</v>
+        <v>2.0269129436259301</v>
       </c>
       <c r="D5">
         <v>2.00587260674684</v>
       </c>
       <c r="E5">
-        <v>1.4975517866132</v>
+        <v>1.5262150524318701</v>
       </c>
       <c r="F5">
-        <v>1.4978511494435001</v>
+        <v>1.5054790951119701</v>
       </c>
       <c r="G5">
-        <v>0.99893169774885604</v>
+        <v>1.00535569580512</v>
       </c>
       <c r="H5">
-        <v>0.99839969445937804</v>
+        <v>0.97550431478145905</v>
       </c>
       <c r="I5">
-        <v>0.59903215869149296</v>
+        <v>1.0081890395142601</v>
       </c>
       <c r="J5">
-        <v>0.49919209712172702</v>
+        <v>0.50540244401992596</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6774,35 +6774,35 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <f>AVERAGE(C4:D5)</f>
-        <v>1.9994849826875072</v>
+        <v>1.9992018047064173</v>
       </c>
       <c r="D8">
         <f>_xlfn.STDEV.S(C4:D5)</f>
-        <v>4.2601461144781607E-3</v>
+        <v>2.1777479237893492E-2</v>
       </c>
       <c r="E8">
         <f>AVERAGE(E4:F5)</f>
-        <v>1.510795362794785</v>
+        <v>1.5148896239359775</v>
       </c>
       <c r="F8">
         <f>_xlfn.STDEV.S(E4:F5)</f>
-        <v>2.5997479709529869E-2</v>
+        <v>3.0497616737153389E-2</v>
       </c>
       <c r="G8">
         <f>AVERAGE(G4:H5)</f>
-        <v>0.99871872756736235</v>
+        <v>0.98834065360685797</v>
       </c>
       <c r="H8">
         <f>_xlfn.STDEV.S(G4:H5)</f>
-        <v>2.7858533996331399E-4</v>
+        <v>1.9157909326553625E-2</v>
       </c>
       <c r="I8">
         <f>AVERAGE(I4:J5)</f>
-        <v>0.52422870179434278</v>
+        <v>0.65168024188710472</v>
       </c>
       <c r="J8">
         <f>_xlfn.STDEV.S(I4:J5)</f>
-        <v>4.9869100992872242E-2</v>
+        <v>0.26310586709748757</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
stopping point for final report + pres
</commit_message>
<xml_diff>
--- a/algorithm proto/results.xlsx
+++ b/algorithm proto/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Desktop\school\capstone\capstone code\algorithm proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210FB5F8-C306-4CBC-A907-311887F7689A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD5F56A-CAC9-4E40-A834-7BDA9D63CC48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1560" windowWidth="20730" windowHeight="11160" xr2:uid="{5F0FE87E-33D9-4A6C-ACD6-13EF39E57134}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0FE87E-33D9-4A6C-ACD6-13EF39E57134}"/>
   </bookViews>
   <sheets>
     <sheet name="frequency" sheetId="1" r:id="rId1"/>
@@ -719,6 +719,33 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Measured Frequency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Applied Frequency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -734,10 +761,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -766,19 +790,70 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.31484689413823275"/>
+                  <c:y val="6.2912510936132982E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -904,6 +979,8 @@
         <c:axId val="311094200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.2000000000000002"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -921,6 +998,60 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Applied</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> Frequency (Hz)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -943,12 +1074,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -966,6 +1094,8 @@
         <c:axId val="304075248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.2000000000000002"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -983,6 +1113,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Measured Frequency (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1005,12 +1184,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1063,7 +1239,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -6151,16 +6331,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6643,7 +6823,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>